<commit_message>
Atualização de planilha com dados de projetos
</commit_message>
<xml_diff>
--- a/projetos.xlsx
+++ b/projetos.xlsx
@@ -7,16 +7,14 @@
     <workbookView xWindow="480" yWindow="435" windowWidth="19875" windowHeight="7710"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
-    <sheet name="Plan2" sheetId="2" r:id="rId2"/>
-    <sheet name="Plan3" sheetId="3" r:id="rId3"/>
+    <sheet name="geral" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="51">
   <si>
     <t>Projeto</t>
   </si>
@@ -33,9 +31,6 @@
     <t>Readme</t>
   </si>
   <si>
-    <t>Docs</t>
-  </si>
-  <si>
     <t>Wiki</t>
   </si>
   <si>
@@ -144,17 +139,41 @@
     <t>Ferramenta case ágil para pequenas e médias equipes</t>
   </si>
   <si>
-    <t>Uma página para os meus projetos de análise e desenvolvimento!</t>
-  </si>
-  <si>
     <t>Treinamento e aprendizagem em Git e GitHub</t>
+  </si>
+  <si>
+    <t>MPS</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>DEV</t>
+  </si>
+  <si>
+    <t>Portfólio online de projetos de Marcos Silva</t>
+  </si>
+  <si>
+    <t>v1.0.0.0</t>
+  </si>
+  <si>
+    <t>MPS et al.</t>
+  </si>
+  <si>
+    <t>PROT</t>
+  </si>
+  <si>
+    <t>DEMO</t>
+  </si>
+  <si>
+    <t>Doc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,16 +181,48 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99FF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -179,13 +230,53 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -194,6 +285,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF99FF99"/>
+      <color rgb="FFFFFF99"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -491,210 +588,476 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" customWidth="1"/>
-    <col min="2" max="2" width="82.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="2" max="2" width="76.5703125" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="10" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="10">
+        <v>42866</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="10">
+        <v>42849</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C4" s="10">
+        <v>42868</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" s="6"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="10">
+        <v>42786</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="10">
+        <v>42744</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="10">
+        <v>42529</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="11">
+        <v>42881</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J8" s="7"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="11">
+        <v>42524</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="11">
+        <v>42792</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="11">
+        <v>42513</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J11" s="7"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="12">
+        <v>42580</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="12">
+        <v>42802</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="12">
+        <v>42808</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="12">
+        <v>42518</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="12">
+        <v>42525</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B17" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="C17" s="12">
+        <v>42787</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B18" s="4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" t="s">
-        <v>43</v>
-      </c>
+      <c r="C18" s="12">
+        <v>42533</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="J18" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
PNA ganhou diretório DOC
</commit_message>
<xml_diff>
--- a/projetos.xlsx
+++ b/projetos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="51">
   <si>
     <t>Projeto</t>
   </si>
@@ -588,7 +588,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -724,7 +726,9 @@
       <c r="E5" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="6"/>
+      <c r="F5" s="6" t="s">
+        <v>43</v>
+      </c>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6" t="s">

</xml_diff>

<commit_message>
Triz ganhou diretório DOC
</commit_message>
<xml_diff>
--- a/projetos.xlsx
+++ b/projetos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="51">
   <si>
     <t>Projeto</t>
   </si>
@@ -589,7 +589,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,7 +894,9 @@
       <c r="E12" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F12" s="8"/>
+      <c r="F12" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
       <c r="I12" s="8" t="s">

</xml_diff>

<commit_message>
Atualização da descrição do PNA
</commit_message>
<xml_diff>
--- a/projetos.xlsx
+++ b/projetos.xlsx
@@ -133,9 +133,6 @@
     <t>Análise de estratégias para testes de unidade do projeto SIGECOMV</t>
   </si>
   <si>
-    <t>Previsão em Nova Aba é uma bela página para visualização de previsão do tempo</t>
-  </si>
-  <si>
     <t>Ferramenta case ágil para pequenas e médias equipes</t>
   </si>
   <si>
@@ -167,6 +164,9 @@
   </si>
   <si>
     <t>Doc</t>
+  </si>
+  <si>
+    <t>Uma bela página para visualização de Previsão do Tempo</t>
   </si>
 </sst>
 </file>
@@ -589,7 +589,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,7 +617,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G1" s="9" t="s">
         <v>5</v>
@@ -643,19 +643,19 @@
         <v>42866</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -669,19 +669,19 @@
         <v>42849</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -695,18 +695,18 @@
         <v>42868</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J4" s="6"/>
     </row>
@@ -715,27 +715,27 @@
         <v>28</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="C5" s="10">
         <v>42786</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -749,17 +749,17 @@
         <v>42744</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -773,19 +773,19 @@
         <v>42529</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -799,16 +799,16 @@
         <v>42881</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J8" s="7"/>
     </row>
@@ -817,23 +817,23 @@
         <v>30</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9" s="11">
         <v>42524</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -852,10 +852,10 @@
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -863,7 +863,7 @@
         <v>31</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" s="11">
         <v>42513</v>
@@ -874,7 +874,7 @@
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J11" s="7"/>
     </row>
@@ -883,27 +883,27 @@
         <v>29</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12" s="12">
         <v>42580</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
       <c r="I12" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -918,16 +918,16 @@
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
       <c r="I13" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -941,19 +941,19 @@
         <v>42808</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
       <c r="I14" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -967,19 +967,19 @@
         <v>42518</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
       <c r="I15" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -993,21 +993,21 @@
         <v>42525</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
       <c r="I16" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1021,19 +1021,19 @@
         <v>42787</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
       <c r="I17" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1047,18 +1047,18 @@
         <v>42533</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
       <c r="I18" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J18" s="8"/>
     </row>

</xml_diff>

<commit_message>
Registro do projeto MPSPARKLOT nas listagens
</commit_message>
<xml_diff>
--- a/projetos.xlsx
+++ b/projetos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="53">
   <si>
     <t>Projeto</t>
   </si>
@@ -167,6 +167,12 @@
   </si>
   <si>
     <t>Uma bela página para visualização de Previsão do Tempo</t>
+  </si>
+  <si>
+    <t>mpsparklot</t>
+  </si>
+  <si>
+    <t>Gestor de estacionamentos em Java do início ao fim</t>
   </si>
 </sst>
 </file>
@@ -586,11 +592,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -789,64 +793,68 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="11">
-        <v>42881</v>
-      </c>
-      <c r="D8" s="7" t="s">
+      <c r="A8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="10">
+        <v>42912</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="J8" s="7"/>
+      <c r="E8" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J8" s="6"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="C9" s="11">
-        <v>42524</v>
+        <v>42881</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="7"/>
+      <c r="E9" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="J9" s="7" t="s">
-        <v>42</v>
-      </c>
+      <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="C10" s="11">
-        <v>42792</v>
-      </c>
-      <c r="D10" s="7"/>
+        <v>42524</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>43</v>
+      </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
@@ -860,13 +868,13 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="C11" s="11">
-        <v>42513</v>
+        <v>42792</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -876,51 +884,49 @@
       <c r="I11" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="J11" s="7"/>
+      <c r="J11" s="7" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="12">
-        <v>42580</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>42</v>
-      </c>
+      <c r="A12" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="11">
+        <v>42513</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J12" s="7"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C13" s="12">
-        <v>42802</v>
-      </c>
-      <c r="D13" s="8"/>
+        <v>42580</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>45</v>
+      </c>
       <c r="E13" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="8"/>
+      <c r="F13" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
       <c r="I13" s="8" t="s">
@@ -932,17 +938,15 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C14" s="12">
-        <v>42808</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>47</v>
-      </c>
+        <v>42802</v>
+      </c>
+      <c r="D14" s="8"/>
       <c r="E14" s="8" t="s">
         <v>42</v>
       </c>
@@ -958,13 +962,13 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C15" s="12">
-        <v>42518</v>
+        <v>42808</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>47</v>
@@ -976,7 +980,7 @@
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
       <c r="I15" s="8" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="J15" s="8" t="s">
         <v>42</v>
@@ -984,13 +988,13 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C16" s="12">
-        <v>42525</v>
+        <v>42518</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>47</v>
@@ -998,9 +1002,7 @@
       <c r="E16" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="F16" s="8" t="s">
-        <v>42</v>
-      </c>
+      <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
       <c r="I16" s="8" t="s">
@@ -1012,25 +1014,27 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="C17" s="12">
-        <v>42787</v>
+        <v>42525</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E17" s="8"/>
+      <c r="E17" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="F17" s="8" t="s">
         <v>42</v>
       </c>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
       <c r="I17" s="8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="J17" s="8" t="s">
         <v>42</v>
@@ -1038,29 +1042,55 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="C18" s="12">
-        <v>42533</v>
+        <v>42787</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>42</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="E18" s="8"/>
       <c r="F18" s="8" t="s">
         <v>42</v>
       </c>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
       <c r="I18" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="12">
+        <v>42533</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="J18" s="8"/>
+      <c r="J19" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Desativação da wiki do PTAPP
</commit_message>
<xml_diff>
--- a/projetos.xlsx
+++ b/projetos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="53">
   <si>
     <t>Projeto</t>
   </si>
@@ -594,7 +594,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -781,9 +783,7 @@
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
-      <c r="G7" s="6" t="s">
-        <v>42</v>
-      </c>
+      <c r="G7" s="6"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
Atualização na planilha de projetos
</commit_message>
<xml_diff>
--- a/projetos.xlsx
+++ b/projetos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="56">
   <si>
     <t>Projeto</t>
   </si>
@@ -173,6 +173,15 @@
   </si>
   <si>
     <t>Gestor de estacionamentos em Java do início ao fim</t>
+  </si>
+  <si>
+    <t>elk</t>
+  </si>
+  <si>
+    <t>Apontamentos e exemplos relacionados a plataforma Elastic Stack</t>
+  </si>
+  <si>
+    <t>MIT</t>
   </si>
 </sst>
 </file>
@@ -592,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,64 +828,68 @@
       <c r="J8" s="6"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="11">
-        <v>42881</v>
-      </c>
-      <c r="D9" s="7" t="s">
+      <c r="A9" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="10">
+        <v>42923</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="J9" s="7"/>
+      <c r="E9" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J9" s="6"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="C10" s="11">
-        <v>42524</v>
+        <v>42881</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="7"/>
+      <c r="E10" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="J10" s="7" t="s">
-        <v>42</v>
-      </c>
+      <c r="J10" s="7"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="C11" s="11">
-        <v>42792</v>
-      </c>
-      <c r="D11" s="7"/>
+        <v>42524</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>43</v>
+      </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
@@ -890,13 +903,13 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="C12" s="11">
-        <v>42513</v>
+        <v>42792</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
@@ -906,51 +919,49 @@
       <c r="I12" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="J12" s="7"/>
+      <c r="J12" s="7" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="12">
-        <v>42580</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>42</v>
-      </c>
+      <c r="A13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="11">
+        <v>42513</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J13" s="7"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C14" s="12">
-        <v>42802</v>
-      </c>
-      <c r="D14" s="8"/>
+        <v>42580</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>45</v>
+      </c>
       <c r="E14" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="F14" s="8"/>
+      <c r="F14" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
       <c r="I14" s="8" t="s">
@@ -962,17 +973,15 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C15" s="12">
-        <v>42808</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>47</v>
-      </c>
+        <v>42802</v>
+      </c>
+      <c r="D15" s="8"/>
       <c r="E15" s="8" t="s">
         <v>42</v>
       </c>
@@ -988,13 +997,13 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C16" s="12">
-        <v>42518</v>
+        <v>42808</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>47</v>
@@ -1006,7 +1015,7 @@
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
       <c r="I16" s="8" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="J16" s="8" t="s">
         <v>42</v>
@@ -1014,13 +1023,13 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C17" s="12">
-        <v>42525</v>
+        <v>42518</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>47</v>
@@ -1028,9 +1037,7 @@
       <c r="E17" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="F17" s="8" t="s">
-        <v>42</v>
-      </c>
+      <c r="F17" s="8"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
       <c r="I17" s="8" t="s">
@@ -1042,25 +1049,27 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="C18" s="12">
-        <v>42787</v>
+        <v>42525</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E18" s="8"/>
+      <c r="E18" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="F18" s="8" t="s">
         <v>42</v>
       </c>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
       <c r="I18" s="8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="J18" s="8" t="s">
         <v>42</v>
@@ -1068,29 +1077,55 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="C19" s="12">
-        <v>42533</v>
+        <v>42787</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>42</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="E19" s="8"/>
       <c r="F19" s="8" t="s">
         <v>42</v>
       </c>
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
       <c r="I19" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="12">
+        <v>42533</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="J19" s="8"/>
+      <c r="J20" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Atualização da planilha de projetos
</commit_message>
<xml_diff>
--- a/projetos.xlsx
+++ b/projetos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="60">
   <si>
     <t>Projeto</t>
   </si>
@@ -182,6 +182,18 @@
   </si>
   <si>
     <t>MIT</t>
+  </si>
+  <si>
+    <t>fakesensor</t>
+  </si>
+  <si>
+    <t>pontilhar</t>
+  </si>
+  <si>
+    <t>FKS é uma boa maneira de simular um sensor que produz arquivos de dados</t>
+  </si>
+  <si>
+    <t>Aplicativo web para criação de desenhos com pontos coloridos</t>
   </si>
 </sst>
 </file>
@@ -601,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -851,89 +863,95 @@
       <c r="I9" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="J9" s="6"/>
+      <c r="J9" s="6" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="11">
-        <v>42881</v>
-      </c>
-      <c r="D10" s="7" t="s">
+      <c r="A10" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="10">
+        <v>42928</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="J10" s="7"/>
+      <c r="E10" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J10" s="6"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="11">
-        <v>42524</v>
-      </c>
-      <c r="D11" s="7" t="s">
+      <c r="A11" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="10">
+        <v>42929</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>42</v>
-      </c>
+      <c r="E11" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J11" s="6"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C12" s="11">
-        <v>42792</v>
-      </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
+        <v>42881</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="J12" s="7" t="s">
-        <v>42</v>
-      </c>
+      <c r="J12" s="7"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C13" s="11">
-        <v>42513</v>
-      </c>
-      <c r="D13" s="7"/>
+        <v>42524</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>43</v>
+      </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
@@ -941,77 +959,71 @@
       <c r="I13" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="J13" s="7"/>
+      <c r="J13" s="7" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="12">
-        <v>42580</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="J14" s="8" t="s">
+      <c r="A14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="11">
+        <v>42792</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J14" s="7" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="12">
-        <v>42802</v>
-      </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="J15" s="8" t="s">
-        <v>42</v>
-      </c>
+      <c r="A15" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="11">
+        <v>42513</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J15" s="7"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C16" s="12">
-        <v>42808</v>
+        <v>42580</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="F16" s="8"/>
+      <c r="F16" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
       <c r="I16" s="8" t="s">
@@ -1023,17 +1035,15 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C17" s="12">
-        <v>42518</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>47</v>
-      </c>
+        <v>42802</v>
+      </c>
+      <c r="D17" s="8"/>
       <c r="E17" s="8" t="s">
         <v>42</v>
       </c>
@@ -1041,7 +1051,7 @@
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
       <c r="I17" s="8" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="J17" s="8" t="s">
         <v>42</v>
@@ -1049,13 +1059,13 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C18" s="12">
-        <v>42525</v>
+        <v>42808</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>47</v>
@@ -1063,13 +1073,11 @@
       <c r="E18" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="F18" s="8" t="s">
-        <v>42</v>
-      </c>
+      <c r="F18" s="8"/>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
       <c r="I18" s="8" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="J18" s="8" t="s">
         <v>42</v>
@@ -1077,25 +1085,25 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="C19" s="12">
-        <v>42787</v>
+        <v>42518</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8" t="s">
-        <v>42</v>
-      </c>
+      <c r="E19" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" s="8"/>
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
       <c r="I19" s="8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="J19" s="8" t="s">
         <v>42</v>
@@ -1103,16 +1111,16 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C20" s="12">
-        <v>42533</v>
+        <v>42525</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>42</v>
@@ -1125,7 +1133,61 @@
       <c r="I20" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="J20" s="8"/>
+      <c r="J20" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="12">
+        <v>42787</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="12">
+        <v>42533</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J22" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Atualização da planilha de projetos com XPROMO
</commit_message>
<xml_diff>
--- a/projetos.xlsx
+++ b/projetos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="62">
   <si>
     <t>Projeto</t>
   </si>
@@ -194,6 +194,12 @@
   </si>
   <si>
     <t>Aplicativo web para criação de desenhos com pontos coloridos</t>
+  </si>
+  <si>
+    <t>xpromo</t>
+  </si>
+  <si>
+    <t>Uma rede social de compras coletivas. Explore seu mundo de interesses!</t>
   </si>
 </sst>
 </file>
@@ -613,10 +619,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -916,64 +922,68 @@
       <c r="J11" s="6"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="11">
-        <v>42881</v>
-      </c>
-      <c r="D12" s="7" t="s">
+      <c r="A12" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="10">
+        <v>42932</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="J12" s="7"/>
+      <c r="E12" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="C13" s="11">
-        <v>42524</v>
+        <v>42881</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="7"/>
+      <c r="E13" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="J13" s="7" t="s">
-        <v>42</v>
-      </c>
+      <c r="J13" s="7"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="C14" s="11">
-        <v>42792</v>
-      </c>
-      <c r="D14" s="7"/>
+        <v>42524</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>43</v>
+      </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
@@ -987,13 +997,13 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="C15" s="11">
-        <v>42513</v>
+        <v>42792</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -1003,51 +1013,49 @@
       <c r="I15" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="J15" s="7"/>
+      <c r="J15" s="7" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="12">
-        <v>42580</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>42</v>
-      </c>
+      <c r="A16" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="11">
+        <v>42513</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J16" s="7"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C17" s="12">
-        <v>42802</v>
-      </c>
-      <c r="D17" s="8"/>
+        <v>42580</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>45</v>
+      </c>
       <c r="E17" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="F17" s="8"/>
+      <c r="F17" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
       <c r="I17" s="8" t="s">
@@ -1059,17 +1067,15 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C18" s="12">
-        <v>42808</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>47</v>
-      </c>
+        <v>42802</v>
+      </c>
+      <c r="D18" s="8"/>
       <c r="E18" s="8" t="s">
         <v>42</v>
       </c>
@@ -1085,13 +1091,13 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C19" s="12">
-        <v>42518</v>
+        <v>42808</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>47</v>
@@ -1103,7 +1109,7 @@
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
       <c r="I19" s="8" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="J19" s="8" t="s">
         <v>42</v>
@@ -1111,13 +1117,13 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C20" s="12">
-        <v>42525</v>
+        <v>42518</v>
       </c>
       <c r="D20" s="8" t="s">
         <v>47</v>
@@ -1125,9 +1131,7 @@
       <c r="E20" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="F20" s="8" t="s">
-        <v>42</v>
-      </c>
+      <c r="F20" s="8"/>
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
       <c r="I20" s="8" t="s">
@@ -1139,25 +1143,27 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="C21" s="12">
-        <v>42787</v>
+        <v>42525</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E21" s="8"/>
+      <c r="E21" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="F21" s="8" t="s">
         <v>42</v>
       </c>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
       <c r="I21" s="8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="J21" s="8" t="s">
         <v>42</v>
@@ -1165,29 +1171,55 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="C22" s="12">
-        <v>42533</v>
+        <v>42787</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>42</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="E22" s="8"/>
       <c r="F22" s="8" t="s">
         <v>42</v>
       </c>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
       <c r="I22" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="12">
+        <v>42533</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="J22" s="8"/>
+      <c r="J23" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Atualização da planilha com projeto PROCORTE
</commit_message>
<xml_diff>
--- a/projetos.xlsx
+++ b/projetos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="64">
   <si>
     <t>Projeto</t>
   </si>
@@ -200,6 +200,12 @@
   </si>
   <si>
     <t>Uma rede social de compras coletivas. Explore seu mundo de interesses!</t>
+  </si>
+  <si>
+    <t>procorte</t>
+  </si>
+  <si>
+    <t>Sistema com algoritmos avançados para otimização de problemas de corte</t>
   </si>
 </sst>
 </file>
@@ -619,10 +625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1117,13 +1123,13 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>35</v>
+        <v>63</v>
       </c>
       <c r="C20" s="12">
-        <v>42518</v>
+        <v>42940</v>
       </c>
       <c r="D20" s="8" t="s">
         <v>47</v>
@@ -1137,19 +1143,17 @@
       <c r="I20" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="J20" s="8" t="s">
-        <v>42</v>
-      </c>
+      <c r="J20" s="8"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C21" s="12">
-        <v>42525</v>
+        <v>42518</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>47</v>
@@ -1157,9 +1161,7 @@
       <c r="E21" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="F21" s="8" t="s">
-        <v>42</v>
-      </c>
+      <c r="F21" s="8"/>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
       <c r="I21" s="8" t="s">
@@ -1171,25 +1173,27 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="C22" s="12">
-        <v>42787</v>
+        <v>42525</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E22" s="8"/>
+      <c r="E22" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="F22" s="8" t="s">
         <v>42</v>
       </c>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
       <c r="I22" s="8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="J22" s="8" t="s">
         <v>42</v>
@@ -1197,29 +1201,55 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="C23" s="12">
-        <v>42533</v>
+        <v>42787</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>42</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="E23" s="8"/>
       <c r="F23" s="8" t="s">
         <v>42</v>
       </c>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
       <c r="I23" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="J23" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="12">
+        <v>42533</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="J23" s="8"/>
+      <c r="J24" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>